<commit_message>
Skip almost empty address lines
</commit_message>
<xml_diff>
--- a/test/data/Personen_20141014.xlsx
+++ b/test/data/Personen_20141014.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
   <si>
     <t>GLN Person</t>
   </si>
@@ -95,22 +95,16 @@
     <t>Zürich</t>
   </si>
   <si>
-    <t>7601000295958</t>
-  </si>
-  <si>
-    <t>Christophe Eugène</t>
-  </si>
-  <si>
-    <t>1227</t>
-  </si>
-  <si>
-    <t>Carouge</t>
-  </si>
-  <si>
-    <t>Genf</t>
-  </si>
-  <si>
-    <t>Zahnärztin/Zahnarzt</t>
+    <t>7601000264015</t>
+  </si>
+  <si>
+    <t>Togninalli</t>
+  </si>
+  <si>
+    <t>Danilo</t>
+  </si>
+  <si>
+    <t>Gravesano</t>
   </si>
   <si>
     <t>7601000157638</t>
@@ -262,15 +256,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="7:7"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19:A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.53441295546559"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.53441295546559"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -372,30 +367,30 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="0" t="s">
         <v>28</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>6929</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>29</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="G4" s="0" t="s">
         <v>17</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I4" s="0" t="s">
         <v>19</v>
@@ -406,22 +401,22 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="D5" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="E5" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="F5" s="0" t="s">
         <v>35</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>37</v>
       </c>
       <c r="G5" s="0" t="s">
         <v>17</v>
@@ -438,22 +433,22 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="D6" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="E6" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="F6" s="0" t="s">
         <v>41</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>43</v>
       </c>
       <c r="G6" s="0" t="s">
         <v>17</v>
@@ -470,22 +465,22 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="D7" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="E7" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="F7" s="0" t="s">
         <v>47</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>49</v>
       </c>
       <c r="G7" s="0" t="s">
         <v>17</v>
@@ -500,6 +495,40 @@
         <v>19</v>
       </c>
     </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>